<commit_message>
modify post create user data binding
</commit_message>
<xml_diff>
--- a/Data Files/POST Data/Create User Data.xlsx
+++ b/Data Files/POST Data/Create User Data.xlsx
@@ -4,10 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="valid users" sheetId="2" r:id="rId2"/>
+    <sheet name="invalid users (empty email)" sheetId="3" r:id="rId3"/>
+    <sheet name="invalid users (empty passwords)" sheetId="4" r:id="rId4"/>
+    <sheet name="invalid users (random email)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="104">
   <si>
     <t>no</t>
   </si>
@@ -109,16 +113,253 @@
   </si>
   <si>
     <t>tech architect</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>george.bluth@reqres.in</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Bluth</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/1-image.jpg</t>
+  </si>
+  <si>
+    <t>janet.weaver@reqres.in</t>
+  </si>
+  <si>
+    <t>Janet</t>
+  </si>
+  <si>
+    <t>Weaver</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/2-image.jpg</t>
+  </si>
+  <si>
+    <t>emma.wong@reqres.in</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Wong</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/3-image.jpg</t>
+  </si>
+  <si>
+    <t>eve.holt@reqres.in</t>
+  </si>
+  <si>
+    <t>Eve</t>
+  </si>
+  <si>
+    <t>Holt</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/4-image.jpg</t>
+  </si>
+  <si>
+    <t>charles.morris@reqres.in</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/5-image.jpg</t>
+  </si>
+  <si>
+    <t>tracey.ramos@reqres.in</t>
+  </si>
+  <si>
+    <t>Tracey</t>
+  </si>
+  <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/6-image.jpg</t>
+  </si>
+  <si>
+    <t>michael.lawson@reqres.in</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Lawson</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/7-image.jpg</t>
+  </si>
+  <si>
+    <t>lindsay.ferguson@reqres.in</t>
+  </si>
+  <si>
+    <t>Lindsay</t>
+  </si>
+  <si>
+    <t>Ferguson</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/8-image.jpg</t>
+  </si>
+  <si>
+    <t>tobias.funke@reqres.in</t>
+  </si>
+  <si>
+    <t>Tobias</t>
+  </si>
+  <si>
+    <t>Funke</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/9-image.jpg</t>
+  </si>
+  <si>
+    <t>byron.fields@reqres.in</t>
+  </si>
+  <si>
+    <t>Byron</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/10-image.jpg</t>
+  </si>
+  <si>
+    <t>george.edwards@reqres.in</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/11-image.jpg</t>
+  </si>
+  <si>
+    <t>rachel.howell@reqres.in</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Howell</t>
+  </si>
+  <si>
+    <t>https://reqres.in/img/faces/12-image.jpg</t>
+  </si>
+  <si>
+    <t>mollit</t>
+  </si>
+  <si>
+    <t>reprehenderit</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>consequat</t>
+  </si>
+  <si>
+    <t>dolore</t>
+  </si>
+  <si>
+    <t>nulla</t>
+  </si>
+  <si>
+    <t>minim</t>
+  </si>
+  <si>
+    <t>commodo</t>
+  </si>
+  <si>
+    <t>vellit</t>
+  </si>
+  <si>
+    <t>lorem@gmail.com</t>
+  </si>
+  <si>
+    <t>ipsum@gmail.com</t>
+  </si>
+  <si>
+    <t>dolor@gmail.com</t>
+  </si>
+  <si>
+    <t>sit@gmail.com</t>
+  </si>
+  <si>
+    <t>amet@gmail.com</t>
+  </si>
+  <si>
+    <t>aba</t>
+  </si>
+  <si>
+    <t>casd</t>
+  </si>
+  <si>
+    <t>rwqr513</t>
+  </si>
+  <si>
+    <t>zvzvz</t>
+  </si>
+  <si>
+    <t>qr24q</t>
+  </si>
+  <si>
+    <t>sfasf</t>
+  </si>
+  <si>
+    <t>ghhh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,14 +382,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -614,4 +862,1066 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3:B6" r:id="rId2" display="lorem@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>